<commit_message>
Fix input parser table formatting
</commit_message>
<xml_diff>
--- a/table-formatting/test.xlsx
+++ b/table-formatting/test.xlsx
@@ -548,13 +548,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>109.7451299964792</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.5840038070334835</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
+        <v>109.7451299964792</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.5840038070334835</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>109.7451299964792</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.5840038070334835</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>32</v>
@@ -888,13 +897,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>109.7451299964792</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.5840038070334835</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
+        <v>109.7451299964792</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.5840038070334835</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>109.7451299964792</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.5840038070334835</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Added unit conversion and number of molecule correction.
</commit_message>
<xml_diff>
--- a/table-formatting/test.xlsx
+++ b/table-formatting/test.xlsx
@@ -548,19 +548,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>109.7451299964792</v>
+        <v>26.2297155823325</v>
       </c>
       <c r="C4" s="2">
         <v>0.5840038070334835</v>
       </c>
       <c r="D4" s="2">
-        <v>109.7451299964792</v>
+        <v>26.2297155823325</v>
       </c>
       <c r="E4" s="2">
         <v>0.5840038070334835</v>
       </c>
       <c r="F4" s="2">
-        <v>109.7451299964792</v>
+        <v>26.2297155823325</v>
       </c>
       <c r="G4" s="2">
         <v>0.5840038070334835</v>
@@ -577,19 +577,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>0.9600429514221128</v>
+        <v>9.600429514221128</v>
       </c>
       <c r="C5" s="2">
         <v>0.2985661695337338</v>
       </c>
       <c r="D5" s="2">
-        <v>0.9600429514221128</v>
+        <v>9.600429514221128</v>
       </c>
       <c r="E5" s="2">
         <v>0.2985661695337338</v>
       </c>
       <c r="F5" s="2">
-        <v>0.9600429514221128</v>
+        <v>9.600429514221128</v>
       </c>
       <c r="G5" s="2">
         <v>0.2985661695337338</v>
@@ -603,22 +603,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>0.6713888386566136</v>
+        <v>6.713888386566135</v>
       </c>
       <c r="C6" s="2">
-        <v>0.4990181765615593</v>
+        <v>0.4990181765615594</v>
       </c>
       <c r="D6" s="2">
-        <v>0.6713888386566136</v>
+        <v>6.713888386566135</v>
       </c>
       <c r="E6" s="2">
-        <v>0.4990181765615593</v>
+        <v>0.4990181765615594</v>
       </c>
       <c r="F6" s="2">
-        <v>0.6713888386566136</v>
+        <v>6.713888386566135</v>
       </c>
       <c r="G6" s="2">
-        <v>0.4990181765615593</v>
+        <v>0.4990181765615594</v>
       </c>
       <c r="H6" s="2">
         <v>0.515</v>
@@ -629,22 +629,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>0.7260101054623198</v>
+        <v>7.260101054623197</v>
       </c>
       <c r="C7" s="2">
-        <v>0.3245547642408043</v>
+        <v>0.3245547642408042</v>
       </c>
       <c r="D7" s="2">
-        <v>0.7260101054623198</v>
+        <v>7.260101054623197</v>
       </c>
       <c r="E7" s="2">
-        <v>0.3245547642408043</v>
+        <v>0.3245547642408042</v>
       </c>
       <c r="F7" s="2">
-        <v>0.7260101054623198</v>
+        <v>7.260101054623197</v>
       </c>
       <c r="G7" s="2">
-        <v>0.3245547642408043</v>
+        <v>0.3245547642408042</v>
       </c>
       <c r="H7" s="2">
         <v>1.067</v>
@@ -897,19 +897,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>109.7451299964792</v>
+        <v>26.2297155823325</v>
       </c>
       <c r="C4" s="2">
         <v>0.5840038070334835</v>
       </c>
       <c r="D4" s="2">
-        <v>109.7451299964792</v>
+        <v>26.2297155823325</v>
       </c>
       <c r="E4" s="2">
         <v>0.5840038070334835</v>
       </c>
       <c r="F4" s="2">
-        <v>109.7451299964792</v>
+        <v>26.2297155823325</v>
       </c>
       <c r="G4" s="2">
         <v>0.5840038070334835</v>
@@ -926,19 +926,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>0.9600429514221128</v>
+        <v>9.600429514221128</v>
       </c>
       <c r="C5" s="2">
         <v>0.2985661695337338</v>
       </c>
       <c r="D5" s="2">
-        <v>0.9600429514221128</v>
+        <v>9.600429514221128</v>
       </c>
       <c r="E5" s="2">
         <v>0.2985661695337338</v>
       </c>
       <c r="F5" s="2">
-        <v>0.9600429514221128</v>
+        <v>9.600429514221128</v>
       </c>
       <c r="G5" s="2">
         <v>0.2985661695337338</v>
@@ -952,22 +952,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>0.6713888386566136</v>
+        <v>6.713888386566135</v>
       </c>
       <c r="C6" s="2">
-        <v>0.4990181765615593</v>
+        <v>0.4990181765615594</v>
       </c>
       <c r="D6" s="2">
-        <v>0.6713888386566136</v>
+        <v>6.713888386566135</v>
       </c>
       <c r="E6" s="2">
-        <v>0.4990181765615593</v>
+        <v>0.4990181765615594</v>
       </c>
       <c r="F6" s="2">
-        <v>0.6713888386566136</v>
+        <v>6.713888386566135</v>
       </c>
       <c r="G6" s="2">
-        <v>0.4990181765615593</v>
+        <v>0.4990181765615594</v>
       </c>
       <c r="H6" s="2">
         <v>0.515</v>
@@ -978,22 +978,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>0.7260101054623198</v>
+        <v>7.260101054623197</v>
       </c>
       <c r="C7" s="2">
-        <v>0.3245547642408043</v>
+        <v>0.3245547642408042</v>
       </c>
       <c r="D7" s="2">
-        <v>0.7260101054623198</v>
+        <v>7.260101054623197</v>
       </c>
       <c r="E7" s="2">
-        <v>0.3245547642408043</v>
+        <v>0.3245547642408042</v>
       </c>
       <c r="F7" s="2">
-        <v>0.7260101054623198</v>
+        <v>7.260101054623197</v>
       </c>
       <c r="G7" s="2">
-        <v>0.3245547642408043</v>
+        <v>0.3245547642408042</v>
       </c>
       <c r="H7" s="2">
         <v>1.067</v>

</xml_diff>

<commit_message>
Bug fix parse energy.xvg file
</commit_message>
<xml_diff>
--- a/table-formatting/test.xlsx
+++ b/table-formatting/test.xlsx
@@ -548,22 +548,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>26.2297155823325</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.5840038070334835</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>26.2297155823325</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.5840038070334835</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>26.2297155823325</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.5840038070334835</v>
+        <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>32</v>
@@ -897,22 +888,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>26.2297155823325</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.5840038070334835</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>26.2297155823325</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.5840038070334835</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>26.2297155823325</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.5840038070334835</v>
+        <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>32</v>

</xml_diff>